<commit_message>
add prev adjustments to FP
</commit_message>
<xml_diff>
--- a/Prototype/evaluation.xlsx
+++ b/Prototype/evaluation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217128F-7E14-49CF-95D5-72C4A74BC901}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1C28D6-462C-47B0-9EC6-B785229BA70B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1100" windowWidth="13700" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,47 +20,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Jacky/Philipp</t>
   </si>
   <si>
-    <t>OS</t>
-  </si>
-  <si>
     <t>Edge</t>
   </si>
   <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>Window 10 Home Build 1803</t>
-  </si>
-  <si>
     <t>Firefox</t>
   </si>
   <si>
-    <t xml:space="preserve">Opera </t>
-  </si>
-  <si>
     <t>Safari</t>
   </si>
   <si>
     <t>72.0.3626.109</t>
   </si>
   <si>
-    <t>72.0.3626.119</t>
-  </si>
-  <si>
-    <t>Grafikkarte</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>64bit</t>
-  </si>
-  <si>
     <t>NVIDA GTX 1050</t>
   </si>
   <si>
@@ -73,9 +52,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>auf allen Browsern</t>
-  </si>
-  <si>
     <t>Me</t>
   </si>
   <si>
@@ -85,7 +61,58 @@
     <t>Intel(R) HD Graphics 520</t>
   </si>
   <si>
-    <t>Windows 10 Home Build</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Self Build, 64 bit</t>
+  </si>
+  <si>
+    <t>Acer Swift3, 64 bit</t>
+  </si>
+  <si>
+    <t>Graphic Card</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Windows 10 Home, Build 1803</t>
+  </si>
+  <si>
+    <t>Nadine</t>
+  </si>
+  <si>
+    <t>Samsung, 64 bit</t>
+  </si>
+  <si>
+    <t>Windows 8</t>
+  </si>
+  <si>
+    <t>18.03.2019 (09:17)</t>
+  </si>
+  <si>
+    <t>05.03.2019 (10:53)</t>
+  </si>
+  <si>
+    <t>06.03.2019 (09:36)</t>
+  </si>
+  <si>
+    <t>72.0.3626.121</t>
+  </si>
+  <si>
+    <t>17.17134</t>
+  </si>
+  <si>
+    <t>18.03.2019 (09:20)</t>
+  </si>
+  <si>
+    <t>65.0.2</t>
+  </si>
+  <si>
+    <t>auf 2 tabellen (eine pro technik) aufteilen</t>
   </si>
 </sst>
 </file>
@@ -101,15 +128,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,12 +150,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -403,115 +460,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11" style="1"/>
+    <col min="5" max="7" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11" style="1"/>
+    <col min="11" max="11" width="37.453125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17.171340000000001</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>17.171340000000001</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>17.171340000000001</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>